<commit_message>
updates to code based on in-person demo
</commit_message>
<xml_diff>
--- a/merge_samples_with_btl/IEPAug2023/20240122 IEPAug23.A.xlsx
+++ b/merge_samples_with_btl/IEPAug2023/20240122 IEPAug23.A.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccm21008\Documents\GitHub\gbl_matlab_tools\merge_samples_with_btl\IEPAug2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8FE128-FE18-4922-86D7-E5F43F89668B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B197C79-D72D-4F56-B13B-0000C010D81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="2565" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="945" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="8" r:id="rId1"/>
     <sheet name="all results" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId3"/>
-    <sheet name="standard data" sheetId="4" r:id="rId4"/>
-    <sheet name="headspace data" sheetId="5" r:id="rId5"/>
-    <sheet name="CH4 sample calc" sheetId="6" r:id="rId6"/>
-    <sheet name="N2O sample calc" sheetId="7" r:id="rId7"/>
-    <sheet name="CH1" sheetId="2" r:id="rId8"/>
-    <sheet name="CH2" sheetId="3" r:id="rId9"/>
+    <sheet name="standard data" sheetId="4" r:id="rId3"/>
+    <sheet name="headspace data" sheetId="5" r:id="rId4"/>
+    <sheet name="CH4 sample calc" sheetId="6" r:id="rId5"/>
+    <sheet name="N2O sample calc" sheetId="7" r:id="rId6"/>
+    <sheet name="CH1" sheetId="2" r:id="rId7"/>
+    <sheet name="CH2" sheetId="3" r:id="rId8"/>
+    <sheet name="TS import" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="383">
   <si>
     <t>Analysis date</t>
   </si>
@@ -1158,9 +1158,6 @@
   </si>
   <si>
     <t>IEPAug23</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SHBML12</t>
   </si>
   <si>
     <t>Ni5</t>
@@ -8522,854 +8519,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468087FD-4EEC-4D36-8986-00FBBE83882A}">
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" t="s">
-        <v>363</v>
-      </c>
-      <c r="E1">
-        <v>778</v>
-      </c>
-      <c r="F1">
-        <v>12.2521</v>
-      </c>
-      <c r="G1">
-        <v>35.073599999999999</v>
-      </c>
-      <c r="H1">
-        <v>1027.71080356315</v>
-      </c>
-      <c r="I1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E2">
-        <v>756</v>
-      </c>
-      <c r="F2">
-        <v>9.8209999999999997</v>
-      </c>
-      <c r="G2">
-        <v>34.764899999999997</v>
-      </c>
-      <c r="H2">
-        <v>1027.1675465399001</v>
-      </c>
-      <c r="I2" t="s">
-        <v>364</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C3" t="s">
-        <v>364</v>
-      </c>
-      <c r="D3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E3">
-        <v>734</v>
-      </c>
-      <c r="F3">
-        <v>9.6128999999999998</v>
-      </c>
-      <c r="G3">
-        <v>34.742400000000004</v>
-      </c>
-      <c r="H3">
-        <v>1027.38873000133</v>
-      </c>
-      <c r="I3" t="s">
-        <v>364</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C4" t="s">
-        <v>367</v>
-      </c>
-      <c r="D4" t="s">
-        <v>368</v>
-      </c>
-      <c r="E4">
-        <v>781</v>
-      </c>
-      <c r="F4">
-        <v>15.0085</v>
-      </c>
-      <c r="G4">
-        <v>35.4193</v>
-      </c>
-      <c r="H4">
-        <v>1026.8232976934501</v>
-      </c>
-      <c r="I4" t="s">
-        <v>367</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C5" t="s">
-        <v>364</v>
-      </c>
-      <c r="D5" t="s">
-        <v>369</v>
-      </c>
-      <c r="E5">
-        <v>765</v>
-      </c>
-      <c r="F5">
-        <v>11.7636</v>
-      </c>
-      <c r="G5">
-        <v>34.834499999999998</v>
-      </c>
-      <c r="H5">
-        <v>1026.52124466243</v>
-      </c>
-      <c r="I5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D6" t="s">
-        <v>368</v>
-      </c>
-      <c r="E6">
-        <v>681</v>
-      </c>
-      <c r="F6">
-        <v>14.4115</v>
-      </c>
-      <c r="G6">
-        <v>35.310600000000001</v>
-      </c>
-      <c r="H6">
-        <v>1026.74289564689</v>
-      </c>
-      <c r="I6" t="s">
-        <v>370</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C7" t="s">
-        <v>367</v>
-      </c>
-      <c r="D7" t="s">
-        <v>371</v>
-      </c>
-      <c r="E7">
-        <v>782</v>
-      </c>
-      <c r="F7">
-        <v>15.627700000000001</v>
-      </c>
-      <c r="G7">
-        <v>35.4831</v>
-      </c>
-      <c r="H7">
-        <v>1026.33951614851</v>
-      </c>
-      <c r="I7" t="s">
-        <v>367</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C8" t="s">
-        <v>372</v>
-      </c>
-      <c r="D8" t="s">
-        <v>365</v>
-      </c>
-      <c r="E8">
-        <v>664</v>
-      </c>
-      <c r="F8">
-        <v>8.0029000000000003</v>
-      </c>
-      <c r="G8">
-        <v>34.566400000000002</v>
-      </c>
-      <c r="H8">
-        <v>1028.9322459191801</v>
-      </c>
-      <c r="I8" t="s">
-        <v>373</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C9" t="s">
-        <v>370</v>
-      </c>
-      <c r="D9" t="s">
-        <v>363</v>
-      </c>
-      <c r="E9">
-        <v>679</v>
-      </c>
-      <c r="F9">
-        <v>13.275700000000001</v>
-      </c>
-      <c r="G9">
-        <v>35.177799999999998</v>
-      </c>
-      <c r="H9">
-        <v>1027.0063099787001</v>
-      </c>
-      <c r="I9" t="s">
-        <v>370</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C10" t="s">
-        <v>373</v>
-      </c>
-      <c r="D10" t="s">
-        <v>363</v>
-      </c>
-      <c r="E10">
-        <v>663</v>
-      </c>
-      <c r="F10">
-        <v>8.9700000000000006</v>
-      </c>
-      <c r="G10">
-        <v>34.6629</v>
-      </c>
-      <c r="H10">
-        <v>1028.6244425553</v>
-      </c>
-      <c r="I10" t="s">
-        <v>373</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C11" t="s">
-        <v>374</v>
-      </c>
-      <c r="D11" t="s">
-        <v>371</v>
-      </c>
-      <c r="E11">
-        <v>350</v>
-      </c>
-      <c r="F11">
-        <v>12.488799999999999</v>
-      </c>
-      <c r="G11">
-        <v>34.8919</v>
-      </c>
-      <c r="H11">
-        <v>1026.50481516372</v>
-      </c>
-      <c r="I11" t="s">
-        <v>374</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>189</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C12" t="s">
-        <v>375</v>
-      </c>
-      <c r="D12" t="s">
-        <v>365</v>
-      </c>
-      <c r="E12">
-        <v>391</v>
-      </c>
-      <c r="F12">
-        <v>10.130800000000001</v>
-      </c>
-      <c r="G12">
-        <v>34.796599999999998</v>
-      </c>
-      <c r="H12">
-        <v>1027.4963866165899</v>
-      </c>
-      <c r="I12" t="s">
-        <v>375</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C13" t="s">
-        <v>375</v>
-      </c>
-      <c r="D13" t="s">
-        <v>363</v>
-      </c>
-      <c r="E13">
-        <v>394</v>
-      </c>
-      <c r="F13">
-        <v>10.3505</v>
-      </c>
-      <c r="G13">
-        <v>34.822600000000001</v>
-      </c>
-      <c r="H13">
-        <v>1027.3828562189301</v>
-      </c>
-      <c r="I13" t="s">
-        <v>375</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>191</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C14" t="s">
-        <v>376</v>
-      </c>
-      <c r="D14" t="s">
-        <v>365</v>
-      </c>
-      <c r="E14">
-        <v>336</v>
-      </c>
-      <c r="F14">
-        <v>10.8742</v>
-      </c>
-      <c r="G14">
-        <v>34.787399999999998</v>
-      </c>
-      <c r="H14">
-        <v>1026.6972250629001</v>
-      </c>
-      <c r="I14" t="s">
-        <v>376</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C15" t="s">
-        <v>376</v>
-      </c>
-      <c r="D15" t="s">
-        <v>363</v>
-      </c>
-      <c r="E15">
-        <v>354</v>
-      </c>
-      <c r="F15">
-        <v>10.9346</v>
-      </c>
-      <c r="G15">
-        <v>34.788899999999998</v>
-      </c>
-      <c r="H15">
-        <v>1026.6718239059101</v>
-      </c>
-      <c r="I15" t="s">
-        <v>376</v>
-      </c>
-      <c r="J15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B16" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C16" t="s">
-        <v>374</v>
-      </c>
-      <c r="D16" t="s">
-        <v>377</v>
-      </c>
-      <c r="E16">
-        <v>362</v>
-      </c>
-      <c r="F16">
-        <v>9.6488999999999994</v>
-      </c>
-      <c r="G16">
-        <v>34.744599999999998</v>
-      </c>
-      <c r="H16">
-        <v>1027.3570623748799</v>
-      </c>
-      <c r="I16" t="s">
-        <v>374</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17" t="s">
-        <v>371</v>
-      </c>
-      <c r="E17">
-        <v>170</v>
-      </c>
-      <c r="F17">
-        <v>14.503500000000001</v>
-      </c>
-      <c r="G17">
-        <v>35.174399999999999</v>
-      </c>
-      <c r="H17">
-        <v>1026.38713145986</v>
-      </c>
-      <c r="I17" t="s">
-        <v>378</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C18" t="s">
-        <v>374</v>
-      </c>
-      <c r="D18" t="s">
-        <v>366</v>
-      </c>
-      <c r="E18">
-        <v>351</v>
-      </c>
-      <c r="F18">
-        <v>9.6135999999999999</v>
-      </c>
-      <c r="G18">
-        <v>34.740499999999997</v>
-      </c>
-      <c r="H18">
-        <v>1027.49253436506</v>
-      </c>
-      <c r="I18" t="s">
-        <v>374</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>196</v>
-      </c>
-      <c r="B19" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C19" t="s">
-        <v>374</v>
-      </c>
-      <c r="D19" t="s">
-        <v>369</v>
-      </c>
-      <c r="E19">
-        <v>359</v>
-      </c>
-      <c r="F19">
-        <v>12.4922</v>
-      </c>
-      <c r="G19">
-        <v>34.893099999999997</v>
-      </c>
-      <c r="H19">
-        <v>1026.41943123745</v>
-      </c>
-      <c r="I19" t="s">
-        <v>374</v>
-      </c>
-      <c r="J19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C20" t="s">
-        <v>379</v>
-      </c>
-      <c r="D20" t="s">
-        <v>371</v>
-      </c>
-      <c r="E20">
-        <v>439</v>
-      </c>
-      <c r="F20">
-        <v>13.7158</v>
-      </c>
-      <c r="G20">
-        <v>34.950400000000002</v>
-      </c>
-      <c r="H20">
-        <v>1026.2252622723399</v>
-      </c>
-      <c r="I20" t="s">
-        <v>379</v>
-      </c>
-      <c r="J20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C21" t="s">
-        <v>378</v>
-      </c>
-      <c r="D21" t="s">
-        <v>366</v>
-      </c>
-      <c r="E21">
-        <v>279</v>
-      </c>
-      <c r="F21">
-        <v>4.3593999999999999</v>
-      </c>
-      <c r="G21">
-        <v>34.445900000000002</v>
-      </c>
-      <c r="H21">
-        <v>1031.2035169407</v>
-      </c>
-      <c r="I21" t="s">
-        <v>378</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C22" t="s">
-        <v>380</v>
-      </c>
-      <c r="D22" t="s">
-        <v>363</v>
-      </c>
-      <c r="E22">
-        <v>342</v>
-      </c>
-      <c r="F22">
-        <v>11.244</v>
-      </c>
-      <c r="G22">
-        <v>34.915100000000002</v>
-      </c>
-      <c r="H22">
-        <v>1027.0187519741701</v>
-      </c>
-      <c r="I22" t="s">
-        <v>380</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>200</v>
-      </c>
-      <c r="B23" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C23" t="s">
-        <v>381</v>
-      </c>
-      <c r="D23" t="s">
-        <v>382</v>
-      </c>
-      <c r="E23">
-        <v>314</v>
-      </c>
-      <c r="F23">
-        <v>14.6035</v>
-      </c>
-      <c r="G23">
-        <v>35.133899999999997</v>
-      </c>
-      <c r="H23">
-        <v>1026.1819625715</v>
-      </c>
-      <c r="I23" t="s">
-        <v>381</v>
-      </c>
-      <c r="J23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>201</v>
-      </c>
-      <c r="B24" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C24" t="s">
-        <v>383</v>
-      </c>
-      <c r="D24" t="s">
-        <v>363</v>
-      </c>
-      <c r="E24">
-        <v>293</v>
-      </c>
-      <c r="F24">
-        <v>12.3954</v>
-      </c>
-      <c r="G24">
-        <v>35.044800000000002</v>
-      </c>
-      <c r="H24">
-        <v>1027.0809086952499</v>
-      </c>
-      <c r="I24" t="s">
-        <v>383</v>
-      </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C25" t="s">
-        <v>380</v>
-      </c>
-      <c r="D25" t="s">
-        <v>371</v>
-      </c>
-      <c r="E25">
-        <v>369</v>
-      </c>
-      <c r="F25">
-        <v>13.206099999999999</v>
-      </c>
-      <c r="G25">
-        <v>34.949199999999998</v>
-      </c>
-      <c r="H25">
-        <v>1026.4066509627801</v>
-      </c>
-      <c r="I25" t="s">
-        <v>380</v>
-      </c>
-      <c r="J25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>361</v>
-      </c>
-      <c r="C26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D26" t="s">
-        <v>369</v>
-      </c>
-      <c r="E26">
-        <v>312</v>
-      </c>
-      <c r="F26">
-        <v>14.3375</v>
-      </c>
-      <c r="G26">
-        <v>35.130099999999999</v>
-      </c>
-      <c r="H26">
-        <v>1026.30398785393</v>
-      </c>
-      <c r="I26" t="s">
-        <v>381</v>
-      </c>
-      <c r="J26">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E12D133-94AB-4C88-91E2-98C5BBD35934}">
   <dimension ref="A1:I177"/>
   <sheetViews>
@@ -11051,12 +10200,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91871A7-5432-40D6-8CA2-70DF5C51E63B}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A4" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B34" sqref="B5:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13183,12 +12332,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFCCCE8-39D6-43FA-9D3F-5CF5894F0D54}">
   <dimension ref="A1:AM964"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:J36"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17716,10 +16865,11 @@
     <mergeCell ref="S3:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D358783-6A9F-4AFE-A89C-6E5AC0BA5411}">
   <dimension ref="A1:AL939"/>
   <sheetViews>
@@ -23257,7 +22407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA03D520-EDB7-480C-B86E-4C4B0E3C7316}">
   <dimension ref="A1:U55"/>
   <sheetViews>
@@ -26356,7 +25506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353B418D-255B-42C7-9A1A-CB004F0419EE}">
   <dimension ref="A1:AA55"/>
   <sheetViews>
@@ -30278,4 +29428,852 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468087FD-4EEC-4D36-8986-00FBBE83882A}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1">
+        <v>778</v>
+      </c>
+      <c r="F1">
+        <v>12.2521</v>
+      </c>
+      <c r="G1">
+        <v>35.073599999999999</v>
+      </c>
+      <c r="H1">
+        <v>1027.71080356315</v>
+      </c>
+      <c r="I1" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E2">
+        <v>756</v>
+      </c>
+      <c r="F2">
+        <v>9.8209999999999997</v>
+      </c>
+      <c r="G2">
+        <v>34.764899999999997</v>
+      </c>
+      <c r="H2">
+        <v>1027.1675465399001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>363</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E3">
+        <v>734</v>
+      </c>
+      <c r="F3">
+        <v>9.6128999999999998</v>
+      </c>
+      <c r="G3">
+        <v>34.742400000000004</v>
+      </c>
+      <c r="H3">
+        <v>1027.38873000133</v>
+      </c>
+      <c r="I3" t="s">
+        <v>363</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4">
+        <v>781</v>
+      </c>
+      <c r="F4">
+        <v>15.0085</v>
+      </c>
+      <c r="G4">
+        <v>35.4193</v>
+      </c>
+      <c r="H4">
+        <v>1026.8232976934501</v>
+      </c>
+      <c r="I4" t="s">
+        <v>366</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E5">
+        <v>765</v>
+      </c>
+      <c r="F5">
+        <v>11.7636</v>
+      </c>
+      <c r="G5">
+        <v>34.834499999999998</v>
+      </c>
+      <c r="H5">
+        <v>1026.52124466243</v>
+      </c>
+      <c r="I5" t="s">
+        <v>363</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>367</v>
+      </c>
+      <c r="E6">
+        <v>681</v>
+      </c>
+      <c r="F6">
+        <v>14.4115</v>
+      </c>
+      <c r="G6">
+        <v>35.310600000000001</v>
+      </c>
+      <c r="H6">
+        <v>1026.74289564689</v>
+      </c>
+      <c r="I6" t="s">
+        <v>369</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" t="s">
+        <v>370</v>
+      </c>
+      <c r="E7">
+        <v>782</v>
+      </c>
+      <c r="F7">
+        <v>15.627700000000001</v>
+      </c>
+      <c r="G7">
+        <v>35.4831</v>
+      </c>
+      <c r="H7">
+        <v>1026.33951614851</v>
+      </c>
+      <c r="I7" t="s">
+        <v>366</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D8" t="s">
+        <v>364</v>
+      </c>
+      <c r="E8">
+        <v>664</v>
+      </c>
+      <c r="F8">
+        <v>8.0029000000000003</v>
+      </c>
+      <c r="G8">
+        <v>34.566400000000002</v>
+      </c>
+      <c r="H8">
+        <v>1028.9322459191801</v>
+      </c>
+      <c r="I8" t="s">
+        <v>372</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" t="s">
+        <v>369</v>
+      </c>
+      <c r="D9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E9">
+        <v>679</v>
+      </c>
+      <c r="F9">
+        <v>13.275700000000001</v>
+      </c>
+      <c r="G9">
+        <v>35.177799999999998</v>
+      </c>
+      <c r="H9">
+        <v>1027.0063099787001</v>
+      </c>
+      <c r="I9" t="s">
+        <v>369</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10">
+        <v>663</v>
+      </c>
+      <c r="F10">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="G10">
+        <v>34.6629</v>
+      </c>
+      <c r="H10">
+        <v>1028.6244425553</v>
+      </c>
+      <c r="I10" t="s">
+        <v>372</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D11" t="s">
+        <v>370</v>
+      </c>
+      <c r="E11">
+        <v>350</v>
+      </c>
+      <c r="F11">
+        <v>12.488799999999999</v>
+      </c>
+      <c r="G11">
+        <v>34.8919</v>
+      </c>
+      <c r="H11">
+        <v>1026.50481516372</v>
+      </c>
+      <c r="I11" t="s">
+        <v>373</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D12" t="s">
+        <v>364</v>
+      </c>
+      <c r="E12">
+        <v>391</v>
+      </c>
+      <c r="F12">
+        <v>10.130800000000001</v>
+      </c>
+      <c r="G12">
+        <v>34.796599999999998</v>
+      </c>
+      <c r="H12">
+        <v>1027.4963866165899</v>
+      </c>
+      <c r="I12" t="s">
+        <v>374</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D13" t="s">
+        <v>362</v>
+      </c>
+      <c r="E13">
+        <v>394</v>
+      </c>
+      <c r="F13">
+        <v>10.3505</v>
+      </c>
+      <c r="G13">
+        <v>34.822600000000001</v>
+      </c>
+      <c r="H13">
+        <v>1027.3828562189301</v>
+      </c>
+      <c r="I13" t="s">
+        <v>374</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C14" t="s">
+        <v>375</v>
+      </c>
+      <c r="D14" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14">
+        <v>336</v>
+      </c>
+      <c r="F14">
+        <v>10.8742</v>
+      </c>
+      <c r="G14">
+        <v>34.787399999999998</v>
+      </c>
+      <c r="H14">
+        <v>1026.6972250629001</v>
+      </c>
+      <c r="I14" t="s">
+        <v>375</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C15" t="s">
+        <v>375</v>
+      </c>
+      <c r="D15" t="s">
+        <v>362</v>
+      </c>
+      <c r="E15">
+        <v>354</v>
+      </c>
+      <c r="F15">
+        <v>10.9346</v>
+      </c>
+      <c r="G15">
+        <v>34.788899999999998</v>
+      </c>
+      <c r="H15">
+        <v>1026.6718239059101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>375</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C16" t="s">
+        <v>373</v>
+      </c>
+      <c r="D16" t="s">
+        <v>376</v>
+      </c>
+      <c r="E16">
+        <v>362</v>
+      </c>
+      <c r="F16">
+        <v>9.6488999999999994</v>
+      </c>
+      <c r="G16">
+        <v>34.744599999999998</v>
+      </c>
+      <c r="H16">
+        <v>1027.3570623748799</v>
+      </c>
+      <c r="I16" t="s">
+        <v>373</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C17" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" t="s">
+        <v>370</v>
+      </c>
+      <c r="E17">
+        <v>170</v>
+      </c>
+      <c r="F17">
+        <v>14.503500000000001</v>
+      </c>
+      <c r="G17">
+        <v>35.174399999999999</v>
+      </c>
+      <c r="H17">
+        <v>1026.38713145986</v>
+      </c>
+      <c r="I17" t="s">
+        <v>377</v>
+      </c>
+      <c r="J17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C18" t="s">
+        <v>373</v>
+      </c>
+      <c r="D18" t="s">
+        <v>365</v>
+      </c>
+      <c r="E18">
+        <v>351</v>
+      </c>
+      <c r="F18">
+        <v>9.6135999999999999</v>
+      </c>
+      <c r="G18">
+        <v>34.740499999999997</v>
+      </c>
+      <c r="H18">
+        <v>1027.49253436506</v>
+      </c>
+      <c r="I18" t="s">
+        <v>373</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" t="s">
+        <v>373</v>
+      </c>
+      <c r="D19" t="s">
+        <v>368</v>
+      </c>
+      <c r="E19">
+        <v>359</v>
+      </c>
+      <c r="F19">
+        <v>12.4922</v>
+      </c>
+      <c r="G19">
+        <v>34.893099999999997</v>
+      </c>
+      <c r="H19">
+        <v>1026.41943123745</v>
+      </c>
+      <c r="I19" t="s">
+        <v>373</v>
+      </c>
+      <c r="J19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C20" t="s">
+        <v>378</v>
+      </c>
+      <c r="D20" t="s">
+        <v>370</v>
+      </c>
+      <c r="E20">
+        <v>439</v>
+      </c>
+      <c r="F20">
+        <v>13.7158</v>
+      </c>
+      <c r="G20">
+        <v>34.950400000000002</v>
+      </c>
+      <c r="H20">
+        <v>1026.2252622723399</v>
+      </c>
+      <c r="I20" t="s">
+        <v>378</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C21" t="s">
+        <v>377</v>
+      </c>
+      <c r="D21" t="s">
+        <v>365</v>
+      </c>
+      <c r="E21">
+        <v>279</v>
+      </c>
+      <c r="F21">
+        <v>4.3593999999999999</v>
+      </c>
+      <c r="G21">
+        <v>34.445900000000002</v>
+      </c>
+      <c r="H21">
+        <v>1031.2035169407</v>
+      </c>
+      <c r="I21" t="s">
+        <v>377</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" t="s">
+        <v>379</v>
+      </c>
+      <c r="D22" t="s">
+        <v>362</v>
+      </c>
+      <c r="E22">
+        <v>342</v>
+      </c>
+      <c r="F22">
+        <v>11.244</v>
+      </c>
+      <c r="G22">
+        <v>34.915100000000002</v>
+      </c>
+      <c r="H22">
+        <v>1027.0187519741701</v>
+      </c>
+      <c r="I22" t="s">
+        <v>379</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C23" t="s">
+        <v>380</v>
+      </c>
+      <c r="D23" t="s">
+        <v>381</v>
+      </c>
+      <c r="E23">
+        <v>314</v>
+      </c>
+      <c r="F23">
+        <v>14.6035</v>
+      </c>
+      <c r="G23">
+        <v>35.133899999999997</v>
+      </c>
+      <c r="H23">
+        <v>1026.1819625715</v>
+      </c>
+      <c r="I23" t="s">
+        <v>380</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C24" t="s">
+        <v>382</v>
+      </c>
+      <c r="D24" t="s">
+        <v>362</v>
+      </c>
+      <c r="E24">
+        <v>293</v>
+      </c>
+      <c r="F24">
+        <v>12.3954</v>
+      </c>
+      <c r="G24">
+        <v>35.044800000000002</v>
+      </c>
+      <c r="H24">
+        <v>1027.0809086952499</v>
+      </c>
+      <c r="I24" t="s">
+        <v>382</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E25">
+        <v>369</v>
+      </c>
+      <c r="F25">
+        <v>13.206099999999999</v>
+      </c>
+      <c r="G25">
+        <v>34.949199999999998</v>
+      </c>
+      <c r="H25">
+        <v>1026.4066509627801</v>
+      </c>
+      <c r="I25" t="s">
+        <v>379</v>
+      </c>
+      <c r="J25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C26" t="s">
+        <v>380</v>
+      </c>
+      <c r="D26" t="s">
+        <v>368</v>
+      </c>
+      <c r="E26">
+        <v>312</v>
+      </c>
+      <c r="F26">
+        <v>14.3375</v>
+      </c>
+      <c r="G26">
+        <v>35.130099999999999</v>
+      </c>
+      <c r="H26">
+        <v>1026.30398785393</v>
+      </c>
+      <c r="I26" t="s">
+        <v>380</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>